<commit_message>
v0.4.6 Improved axis scaling
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbeyer/work/ddorf/code/ExcelPlotter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2091B5A6-3DCC-214E-873A-96911132E7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09194B32-2C41-CD42-B4B8-89D128DB1A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="880" windowWidth="32860" windowHeight="22500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3080" yWindow="880" windowWidth="32860" windowHeight="22500" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEAP_TwoGroups" sheetId="17" r:id="rId1"/>
@@ -25,9 +25,10 @@
     <sheet name="Ungrouped_4xcat" sheetId="21" r:id="rId10"/>
     <sheet name="TimeCourse" sheetId="6" r:id="rId11"/>
     <sheet name="XY_single" sheetId="8" r:id="rId12"/>
-    <sheet name="XY_tripple" sheetId="12" r:id="rId13"/>
-    <sheet name="DoseResponse_grouped" sheetId="10" r:id="rId14"/>
-    <sheet name="DoseResponse_columns" sheetId="11" r:id="rId15"/>
+    <sheet name="XY_single_log" sheetId="22" r:id="rId13"/>
+    <sheet name="XY_tripple" sheetId="12" r:id="rId14"/>
+    <sheet name="DoseResponse_grouped" sheetId="10" r:id="rId15"/>
+    <sheet name="DoseResponse_columns" sheetId="11" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="49">
   <si>
     <t>A</t>
   </si>
@@ -244,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,6 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1664,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4750FFA1-D470-3E41-AF67-62D07304E227}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
@@ -4005,6 +4007,96 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2975F59-EC08-734E-BB04-5A1B391B2181}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFFEF0A-7F0D-9A46-84E4-997D6A77EF02}">
   <dimension ref="A1:B63"/>
   <sheetViews>
@@ -4510,18 +4602,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35771B40-B55D-0146-9B05-9D0ACBA527AD}">
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
@@ -4535,7 +4630,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -4549,7 +4644,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>0.1</v>
       </c>
       <c r="B3" t="s">
@@ -4563,7 +4658,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
@@ -4577,7 +4672,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -4591,7 +4686,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -4605,7 +4700,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="10">
         <v>10</v>
       </c>
       <c r="B7" t="s">
@@ -4619,7 +4714,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="10">
         <v>30</v>
       </c>
       <c r="B8" t="s">
@@ -4633,7 +4728,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="10">
         <v>100</v>
       </c>
       <c r="B9" t="s">
@@ -4647,7 +4742,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="10">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -4661,7 +4756,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="10">
         <v>0.1</v>
       </c>
       <c r="B11" t="s">
@@ -4675,7 +4770,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="10">
         <v>0.3</v>
       </c>
       <c r="B12" t="s">
@@ -4689,7 +4784,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="A13" s="10">
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -4703,7 +4798,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="A14" s="10">
         <v>3</v>
       </c>
       <c r="B14" t="s">
@@ -4717,7 +4812,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="A15" s="10">
         <v>10</v>
       </c>
       <c r="B15" t="s">
@@ -4731,7 +4826,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="10">
         <v>30</v>
       </c>
       <c r="B16" t="s">
@@ -4745,7 +4840,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="10">
         <v>100</v>
       </c>
       <c r="B17" t="s">
@@ -4759,7 +4854,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="10">
         <v>0</v>
       </c>
       <c r="B18" t="s">
@@ -4773,7 +4868,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="10">
         <v>0.1</v>
       </c>
       <c r="B19" t="s">
@@ -4787,7 +4882,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="A20" s="10">
         <v>0.3</v>
       </c>
       <c r="B20" t="s">
@@ -4801,7 +4896,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="A21" s="10">
         <v>1</v>
       </c>
       <c r="B21" t="s">
@@ -4815,7 +4910,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="A22" s="10">
         <v>3</v>
       </c>
       <c r="B22" t="s">
@@ -4829,7 +4924,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="A23" s="10">
         <v>10</v>
       </c>
       <c r="B23" t="s">
@@ -4843,7 +4938,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="10">
         <v>30</v>
       </c>
       <c r="B24" t="s">
@@ -4857,7 +4952,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25">
+      <c r="A25" s="10">
         <v>100</v>
       </c>
       <c r="B25" t="s">
@@ -4871,7 +4966,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26">
+      <c r="A26" s="10">
         <v>0</v>
       </c>
       <c r="B26" t="s">
@@ -4885,7 +4980,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27">
+      <c r="A27" s="10">
         <v>0.1</v>
       </c>
       <c r="B27" t="s">
@@ -4899,7 +4994,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="A28" s="10">
         <v>0.3</v>
       </c>
       <c r="B28" t="s">
@@ -4913,7 +5008,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29">
+      <c r="A29" s="10">
         <v>1</v>
       </c>
       <c r="B29" t="s">
@@ -4927,7 +5022,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30">
+      <c r="A30" s="10">
         <v>3</v>
       </c>
       <c r="B30" t="s">
@@ -4941,7 +5036,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31">
+      <c r="A31" s="10">
         <v>10</v>
       </c>
       <c r="B31" t="s">
@@ -4955,7 +5050,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32">
+      <c r="A32" s="10">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -4969,7 +5064,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33">
+      <c r="A33" s="10">
         <v>100</v>
       </c>
       <c r="B33" t="s">
@@ -4983,7 +5078,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34">
+      <c r="A34" s="10">
         <v>0</v>
       </c>
       <c r="B34" t="s">
@@ -4997,7 +5092,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35">
+      <c r="A35" s="10">
         <v>0.1</v>
       </c>
       <c r="B35" t="s">
@@ -5011,7 +5106,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="A36" s="10">
         <v>0.3</v>
       </c>
       <c r="B36" t="s">
@@ -5025,7 +5120,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37">
+      <c r="A37" s="10">
         <v>1</v>
       </c>
       <c r="B37" t="s">
@@ -5039,7 +5134,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="A38" s="10">
         <v>3</v>
       </c>
       <c r="B38" t="s">
@@ -5053,7 +5148,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="10">
         <v>10</v>
       </c>
       <c r="B39" t="s">
@@ -5067,7 +5162,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="10">
         <v>30</v>
       </c>
       <c r="B40" t="s">
@@ -5081,7 +5176,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="A41" s="10">
         <v>100</v>
       </c>
       <c r="B41" t="s">
@@ -5095,7 +5190,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="10">
         <v>0</v>
       </c>
       <c r="B42" t="s">
@@ -5109,7 +5204,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="A43" s="10">
         <v>0.1</v>
       </c>
       <c r="B43" t="s">
@@ -5123,7 +5218,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="A44" s="10">
         <v>0.3</v>
       </c>
       <c r="B44" t="s">
@@ -5137,7 +5232,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="A45" s="10">
         <v>1</v>
       </c>
       <c r="B45" t="s">
@@ -5151,7 +5246,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="A46" s="10">
         <v>3</v>
       </c>
       <c r="B46" t="s">
@@ -5165,7 +5260,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47">
+      <c r="A47" s="10">
         <v>10</v>
       </c>
       <c r="B47" t="s">
@@ -5179,7 +5274,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48">
+      <c r="A48" s="10">
         <v>30</v>
       </c>
       <c r="B48" t="s">
@@ -5193,7 +5288,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49">
+      <c r="A49" s="10">
         <v>100</v>
       </c>
       <c r="B49" t="s">
@@ -5211,21 +5306,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C923E9B-E81A-804D-8935-FFACD0D86CE7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V61" sqref="V61"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="10"/>
     <col min="3" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
@@ -5239,7 +5335,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -5253,7 +5349,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>0.1</v>
       </c>
       <c r="B3" t="s">
@@ -5267,7 +5363,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
@@ -5281,7 +5377,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -5295,7 +5391,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -5309,7 +5405,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="10">
         <v>10</v>
       </c>
       <c r="B7" t="s">
@@ -5323,7 +5419,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="10">
         <v>30</v>
       </c>
       <c r="B8" t="s">
@@ -5337,7 +5433,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="10">
         <v>100</v>
       </c>
       <c r="B9" t="s">
@@ -5351,7 +5447,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="10">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -5365,7 +5461,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="10">
         <v>0.1</v>
       </c>
       <c r="B11" t="s">
@@ -5379,7 +5475,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="10">
         <v>0.3</v>
       </c>
       <c r="B12" t="s">
@@ -5393,7 +5489,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="A13" s="10">
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -5407,7 +5503,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="A14" s="10">
         <v>3</v>
       </c>
       <c r="B14" t="s">
@@ -5421,7 +5517,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="A15" s="10">
         <v>10</v>
       </c>
       <c r="B15" t="s">
@@ -5435,7 +5531,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="10">
         <v>30</v>
       </c>
       <c r="B16" t="s">
@@ -5449,7 +5545,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="10">
         <v>100</v>
       </c>
       <c r="B17" t="s">
@@ -5463,7 +5559,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="10">
         <v>0</v>
       </c>
       <c r="B18" t="s">
@@ -5477,7 +5573,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="10">
         <v>0.1</v>
       </c>
       <c r="B19" t="s">
@@ -5491,7 +5587,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="A20" s="10">
         <v>0.3</v>
       </c>
       <c r="B20" t="s">
@@ -5505,7 +5601,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="A21" s="10">
         <v>1</v>
       </c>
       <c r="B21" t="s">
@@ -5519,7 +5615,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="A22" s="10">
         <v>3</v>
       </c>
       <c r="B22" t="s">
@@ -5533,7 +5629,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="A23" s="10">
         <v>10</v>
       </c>
       <c r="B23" t="s">
@@ -5547,7 +5643,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="10">
         <v>30</v>
       </c>
       <c r="B24" t="s">
@@ -5561,7 +5657,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25">
+      <c r="A25" s="10">
         <v>100</v>
       </c>
       <c r="B25" t="s">

</xml_diff>

<commit_message>
v0.5.9 Reimplementation of statistics and errorbars
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbeyer/work/ddorf/code/ExcelPlotter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbeyer/work/ddorf/code/ExPlot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10129B44-1C11-6D49-ABBA-259A30C754F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D220D0-D496-8247-8626-9E970BFF7C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="1040" windowWidth="32860" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3140" yWindow="880" windowWidth="32860" windowHeight="22500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEAP_TwoGroups" sheetId="17" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="45">
   <si>
     <t>A</t>
   </si>
@@ -178,7 +178,13 @@
     <t>Dark</t>
   </si>
   <si>
-    <t>SEAP / U-1 L-1</t>
+    <t>SEAP / U$^{-1}$ L$^{-1}$</t>
+  </si>
+  <si>
+    <t>Metric3</t>
+  </si>
+  <si>
+    <t>Metric4</t>
   </si>
 </sst>
 </file>
@@ -553,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BCEB9D-2277-1B4F-9DC4-F45384EB4EB1}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1020,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4750FFA1-D470-3E41-AF67-62D07304E227}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1876,6 +1882,9 @@
       <c r="B106">
         <v>25</v>
       </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" s="1"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
@@ -9578,15 +9587,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3642A00B-427B-6A42-8AE7-8FDA20437EF1}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -9599,8 +9608,14 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -9613,8 +9628,14 @@
       <c r="D2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -9627,8 +9648,14 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -9641,8 +9668,14 @@
       <c r="D4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -9655,8 +9688,14 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -9669,8 +9708,14 @@
       <c r="D6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -9683,8 +9728,14 @@
       <c r="D7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -9697,8 +9748,14 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -9711,8 +9768,14 @@
       <c r="D9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -9725,8 +9788,14 @@
       <c r="D10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -9739,8 +9808,14 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -9753,8 +9828,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -9765,6 +9846,12 @@
         <v>4</v>
       </c>
       <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.7.5 Second Y-axis support,  improved packaging
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbeyer/repos/ExPlot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86A2EE2-1C1A-CD4A-96CD-DE77BAE97629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339D5173-FA9A-024B-93D7-FF17EBF5BECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="780" windowWidth="31900" windowHeight="22600" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="780" windowWidth="31900" windowHeight="22600" firstSheet="12" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEAP_TwoGroups" sheetId="9" r:id="rId1"/>
@@ -33,13 +33,15 @@
     <sheet name="Heatmap_Pivot" sheetId="19" r:id="rId18"/>
     <sheet name="Heatmap_Corr" sheetId="20" r:id="rId19"/>
     <sheet name="Heatmap_DrugScreen" sheetId="18" r:id="rId20"/>
+    <sheet name="DualAxis_Columns" sheetId="22" r:id="rId21"/>
+    <sheet name="DualAxis_Grouped" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="93">
   <si>
     <t>Condition</t>
   </si>
@@ -303,6 +305,21 @@
   </si>
   <si>
     <t>Measurement 2</t>
+  </si>
+  <si>
+    <t>Viability (%)</t>
+  </si>
+  <si>
+    <t>Protein (mg/mL)</t>
+  </si>
+  <si>
+    <t>Absorbance (AU)</t>
+  </si>
+  <si>
+    <t>Cell Line</t>
+  </si>
+  <si>
+    <t>CHO</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -10014,6 +10031,611 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A279C8E4-FB18-3F4A-9BA1-6119DEE349B3}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>98.417727190009515</v>
+      </c>
+      <c r="C2">
+        <v>2.3171366678656748</v>
+      </c>
+      <c r="D2">
+        <v>5.1656317157017823E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>91.08065975224045</v>
+      </c>
+      <c r="C3">
+        <v>2.6030854868705391</v>
+      </c>
+      <c r="D3">
+        <v>0.13487772563561179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>89.343627902203139</v>
+      </c>
+      <c r="C4">
+        <v>2.47108795339118</v>
+      </c>
+      <c r="D4">
+        <v>0.20760412881077361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>89.393722471738243</v>
+      </c>
+      <c r="C5">
+        <v>3.5972251908184378</v>
+      </c>
+      <c r="D5">
+        <v>0.2890717051166809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>87.476933159990821</v>
+      </c>
+      <c r="C6">
+        <v>3.8844753158751049</v>
+      </c>
+      <c r="D6">
+        <v>0.36446832512996991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>83.34273656237994</v>
+      </c>
+      <c r="C7">
+        <v>4.2969233999082128</v>
+      </c>
+      <c r="D7">
+        <v>0.44401896687959658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>79.768703435223514</v>
+      </c>
+      <c r="C8">
+        <v>5.1835028866522608</v>
+      </c>
+      <c r="D8">
+        <v>0.534062629111971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>76.397792608821419</v>
+      </c>
+      <c r="C9">
+        <v>5.809299856748785</v>
+      </c>
+      <c r="D9">
+        <v>0.6167812001428542</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>71.042956019265148</v>
+      </c>
+      <c r="C10">
+        <v>6.2793840357348598</v>
+      </c>
+      <c r="D10">
+        <v>0.68963994939209838</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>69.560311583210577</v>
+      </c>
+      <c r="C11">
+        <v>6.2482347430332084</v>
+      </c>
+      <c r="D11">
+        <v>0.77501766448946019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>67.078722458080421</v>
+      </c>
+      <c r="C12">
+        <v>6.9072362872446353</v>
+      </c>
+      <c r="D12">
+        <v>0.85180818012523829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3817E6B3-7EB6-2D4A-A542-D3DE5BF3C32A}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U53" sqref="U53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>533.90919744193639</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3">
+        <v>0.54706009933035715</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>541.45791669640937</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>0.87931893084619928</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.1</v>
+      </c>
+      <c r="B6">
+        <v>497.3658210552079</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
+        <v>0.52788556817475796</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8">
+        <v>624.94078582294287</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>0.92056618979303595</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.3</v>
+      </c>
+      <c r="B10">
+        <v>522.50642575082566</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.3</v>
+      </c>
+      <c r="B11">
+        <v>0.8755912526796471</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.3</v>
+      </c>
+      <c r="B12">
+        <v>522.80926040695022</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.3</v>
+      </c>
+      <c r="B13">
+        <v>0.67393329324840279</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>754.1838302729152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1.0672736187182561</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>655.83982506896177</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1.337472161801621</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>691.44416067789223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1.512779134168871</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1204.598796223939</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>2.4675392597329422</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>1323.282438446078</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>2.7048447399026929</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>1253.376410234396</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>2.4650503627573088</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>1761.090061227673</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>4.1635477071850646</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>1730.7595185828161</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>4.2165027929122258</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>1758.2772629579911</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>4.0830244392844364</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1923.9345243409571</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>5.1033763929393334</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>1953.3449937155301</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>4.5213785702463651</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>1995.1471005575861</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>4.4887520260433407</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B31"/>

</xml_diff>